<commit_message>
Finished reg ex exercise
</commit_message>
<xml_diff>
--- a/week2/DataManipString/ApplicantInfo.xlsx
+++ b/week2/DataManipString/ApplicantInfo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Batches\230206-UiPath-BNYM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Catherine-Schiber-Code\week2\DataManipString\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C1746E-BC3A-4E79-99AD-9995AD80193C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FE3DBC-5C2E-4E35-9A1A-3DB73A1D78AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2060" yWindow="3230" windowWidth="16800" windowHeight="9670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -494,6 +494,9 @@
       <c r="E2" t="s">
         <v>10</v>
       </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -511,6 +514,9 @@
       <c r="E3" t="s">
         <v>15</v>
       </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -528,6 +534,9 @@
       <c r="E4" t="s">
         <v>20</v>
       </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -545,6 +554,9 @@
       <c r="E5" t="s">
         <v>24</v>
       </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -558,6 +570,9 @@
       </c>
       <c r="D6" t="s">
         <v>29</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -571,6 +586,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010029651A743809674EA380985F8EF857EB" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3a9634b484a8fb32dc6909a8699afd82">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8281136c-3236-4060-8248-b02a7f3e9f10" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb502cd37ece96e68cda9ac896eab4a3" ns2:_="">
     <xsd:import namespace="8281136c-3236-4060-8248-b02a7f3e9f10"/>
@@ -702,19 +726,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08881C51-C8EA-4232-90FB-18F2EB429C8D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A399F8E-2F26-4A9B-ADFC-CDECAF81AB28}"/>
-</file>
-
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08881C51-C8EA-4232-90FB-18F2EB429C8D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A399F8E-2F26-4A9B-ADFC-CDECAF81AB28}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8281136c-3236-4060-8248-b02a7f3e9f10"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Demos for ui path automation.
</commit_message>
<xml_diff>
--- a/week2/DataManipString/ApplicantInfo.xlsx
+++ b/week2/DataManipString/ApplicantInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Catherine-Schiber-Code\week2\DataManipString\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FE3DBC-5C2E-4E35-9A1A-3DB73A1D78AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47806259-FC0D-4BFB-8446-CE1951F02472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="3230" windowWidth="16800" windowHeight="9670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1030" yWindow="2070" windowWidth="16800" windowHeight="9670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -586,15 +586,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010029651A743809674EA380985F8EF857EB" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3a9634b484a8fb32dc6909a8699afd82">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8281136c-3236-4060-8248-b02a7f3e9f10" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb502cd37ece96e68cda9ac896eab4a3" ns2:_="">
     <xsd:import namespace="8281136c-3236-4060-8248-b02a7f3e9f10"/>
@@ -726,15 +717,16 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08881C51-C8EA-4232-90FB-18F2EB429C8D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A399F8E-2F26-4A9B-ADFC-CDECAF81AB28}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -750,4 +742,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08881C51-C8EA-4232-90FB-18F2EB429C8D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>